<commit_message>
is al weer een week geleden
</commit_message>
<xml_diff>
--- a/Documentatie/Time tracking.xlsx
+++ b/Documentatie/Time tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tijss\GitHub\IT-s-in-the-game\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026DCA82-407C-4185-B33B-A3B7067E841F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69042796-137C-4BF3-B6C9-4758771B52FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -769,19 +769,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -855,19 +855,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -941,19 +941,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1027,19 +1027,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1323,28 +1323,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>400</c:v>
+                  <c:v>368</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>395</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>395</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>395</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>395</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>395</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>395</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3519,8 +3519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3768,21 +3768,19 @@
         <v>36</v>
       </c>
       <c r="E2" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G2" s="3">
         <v>5</v>
       </c>
       <c r="H2" s="3">
-        <f>'Week (4)'!$H$11</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I2" s="3">
-        <f>'Week (5)'!$H$11</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J2" s="3">
         <f>'Week (6)'!$H$11</f>
@@ -3798,7 +3796,7 @@
       </c>
       <c r="M2" s="4">
         <f>SUM(E2:L2)</f>
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3808,22 +3806,19 @@
         <v>37</v>
       </c>
       <c r="E3" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G3" s="3">
-        <f>'Week (3)'!$H$21</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H3" s="3">
-        <f>'Week (4)'!$H$21</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I3" s="3">
-        <f>'Week (5)'!$H$21</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J3" s="3">
         <f>'Week (6)'!$H$21</f>
@@ -3839,7 +3834,7 @@
       </c>
       <c r="M3" s="4">
         <f t="shared" ref="M3:M5" si="0">SUM(E3:L3)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3853,22 +3848,19 @@
         <v>38</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4" s="3">
-        <f>'Week (3)'!$H$31</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="3">
-        <f>'Week (4)'!$H$31</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I4" s="3">
-        <f>'Week (5)'!$H$31</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" s="3">
         <f>'Week (6)'!$H$31</f>
@@ -3884,7 +3876,7 @@
       </c>
       <c r="M4" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3894,22 +3886,19 @@
         <v>39</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G5" s="3">
-        <f>'Week (3)'!$H$41</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="3">
-        <f>'Week (4)'!$H$41</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I5" s="3">
-        <f>'Week (5)'!$H$41</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J5" s="3">
         <f>'Week (6)'!$H$41</f>
@@ -3925,7 +3914,7 @@
       </c>
       <c r="M5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -3950,23 +3939,23 @@
       </c>
       <c r="E7" s="15">
         <f t="shared" ref="E7:L7" si="1">SUM(E2:E6)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F7" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G7" s="15">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H7" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I7" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J7" s="15">
         <f t="shared" si="1"/>
@@ -3990,17 +3979,17 @@
       <c r="E8" s="21"/>
       <c r="F8" s="21">
         <f>SUM(E7:F7)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21">
         <f>SUM(G7:H7)</f>
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21">
         <f>SUM(I7:J7)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K8" s="21"/>
       <c r="L8" s="21">
@@ -4016,35 +4005,35 @@
       </c>
       <c r="E9" s="19">
         <f>E10-E7</f>
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="F9" s="19">
         <f>E9-F7</f>
-        <v>400</v>
+        <v>368</v>
       </c>
       <c r="G9" s="19">
         <f t="shared" ref="G9:L9" si="2">F9-G7</f>
-        <v>395</v>
+        <v>350</v>
       </c>
       <c r="H9" s="19">
         <f t="shared" si="2"/>
-        <v>395</v>
+        <v>324</v>
       </c>
       <c r="I9" s="19">
         <f t="shared" si="2"/>
-        <v>395</v>
+        <v>304</v>
       </c>
       <c r="J9" s="19">
         <f t="shared" si="2"/>
-        <v>395</v>
+        <v>304</v>
       </c>
       <c r="K9" s="19">
         <f t="shared" si="2"/>
-        <v>395</v>
+        <v>304</v>
       </c>
       <c r="L9" s="19">
         <f t="shared" si="2"/>
-        <v>395</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -10534,6 +10523,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </c6664f9864b54a78bdf9e6230de1c78b>
+    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100294690D6A57C3C4B8650464765815F1C" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="bf1d2ff51e740e451b46e7c13bf9e6da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45f6ce90-ba85-4ef2-b43f-c64448cd95eb" xmlns:ns3="c7549584-aa9c-449c-abfe-2ca02f3a7188" xmlns:ns4="6c73e52c-07d4-4617-ab67-464747257e8d" xmlns:ns5="ab37b2fe-4f81-426e-b942-40459dbac68c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8575fd65d7959dd12bd4dc11d36e634e" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="45f6ce90-ba85-4ef2-b43f-c64448cd95eb"/>
@@ -10776,17 +10776,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </c6664f9864b54a78bdf9e6230de1c78b>
-    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844B94A5-2CB8-4D3A-A97F-85854BBCA257}">
   <ds:schemaRefs>
@@ -10796,6 +10785,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
+    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{724CCB8E-5E6A-4B8C-A558-5D9223ADF390}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10814,15 +10814,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
-    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>